<commit_message>
update traffic light module
</commit_message>
<xml_diff>
--- a/script/result_llm_tranform/autoware_docs/autoware_behavior_velocity_traffic_light/result.xlsx
+++ b/script/result_llm_tranform/autoware_docs/autoware_behavior_velocity_traffic_light/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26860" windowHeight="15060"/>
+    <workbookView windowWidth="21540" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="mtl" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="74">
   <si>
     <t>index</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>lower than 2.0m/s ⇒ stop</t>
-  </si>
-  <si>
-    <t>{'sentence': 'vehicle can pass through stop line during yellow lamp.(left side of the yellow lamp line)', 'formula': 'Y ∧ P', 'explanation': 'Y represents the yellow lamp being active, and P represents the vehicle passing through the stop line. The conjunction Y ∧ P indicates the vehicle can pass through during the yellow lamp phase.'}</t>
   </si>
   <si>
     <t>When it to be judged that vehicle can’t stop before stop line, autoware chooses one of the following behaviors</t>
@@ -200,11 +197,11 @@
 {'sentence': 'vehicle can pass through stop line during yellow lamp.(left side of the yellow lamp line)', 'formula': 'Y → P', 'explanation': 'Here, Y represents the yellow lamp, and P represents the vehicle passing through the stop line. The formula states that if the yellow lamp is on, the vehicle can pass through the stop line.'}</t>
   </si>
   <si>
-    <t xml:space="preserve">{'sentence': '4.When it to be judged that vehicle can’t stop before stop line, autoware chooses one of the following behaviors', 'formula': '¬R → F(B1 ∨ B2 ∨ B3)', 'explanation': 'R represents the vehicle stopping before the stop line. If this is not possible (¬R), the system eventually chooses one of several behaviors (B1, B2, B3), indicating alternative actions by the autoware.'}
+    <t>{'sentence': '4.When it to be judged that vehicle can’t stop before stop line, autoware chooses one of the following behaviors', 'formula': '¬R → F(B1 ∨ B2 ∨ B3)', 'explanation': 'R represents the vehicle stopping before the stop line. If this is not possible (¬R), the system eventually chooses one of several behaviors (B1, B2, B3), indicating alternative actions by the autoware.'}
 {'sentence': '"can pass through" stop line during yellow lamp =&gt; pass', 'formula': 'Y ∧ C → P', 'explanation': 'Y denotes the yellow lamp active, C indicates the ability to pass through the stop line, and P represents passing. The formula suggests that if passing through during a yellow lamp is possible, it should pass.'}
 {'sentence': '"can’t pass through" stop line during yellow lamp =&gt; emergency stop', 'formula': 'Y ∧ ¬C → E', 'explanation': "Y indicates the yellow lamp, ¬C represents the inability to pass through, and E is an emergency stop. The formula indicates an emergency stop when passing isn't possible during a yellow light."}
 {'sentence': 'vehicle can’t pass through stop line during yellow lamp.(right side of the yellow lamp line)', 'formula': 'Y ∧ ¬C', 'explanation': 'Y represents the yellow lamp, and ¬C denotes being unable to pass through the stop line. This captures the condition where passing is not feasible during the yellow light period.'}
-</t>
+{'sentence': 'vehicle can pass through stop line during yellow lamp.(left side of the yellow lamp line)', 'formula': 'Y ∧ P', 'explanation': 'Y represents the yellow lamp being active, and P represents the vehicle passing through the stop line. The conjunction Y ∧ P indicates the vehicle can pass through during the yellow lamp phase.'}</t>
   </si>
   <si>
     <t>{'sentence': '"can pass through" stop line during yellow lamp =&gt; pass', 'formula': 'G((C ∧ Y) → P)', 'explanation': "C represents 'can pass through stop line', Y represents 'yellow lamp', and P represents 'pass'. This formula states that globally, if the vehicle can pass through the stop line during a yellow lamp, then it's allowed to pass."}
@@ -1256,8 +1253,8 @@
   <sheetPr/>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" topLeftCell="F18" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1559,7 +1556,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" ht="185" spans="1:12">
+    <row r="9" ht="34" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1582,9 +1579,7 @@
       <c r="H9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1604,28 +1599,28 @@
         <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="L10" s="2">
         <v>1</v>
@@ -1642,7 +1637,7 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>7</v>
@@ -1674,7 +1669,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>7</v>
@@ -1703,31 +1698,31 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="L13" s="2">
         <v>1</v>
@@ -1741,31 +1736,31 @@
         <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="L14" s="2">
         <v>1</v>
@@ -1905,7 +1900,7 @@
         <v>7</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H18" s="2">
         <v>0</v>
@@ -1981,7 +1976,7 @@
         <v>7</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>

</xml_diff>